<commit_message>
new graph for hit ratio
</commit_message>
<xml_diff>
--- a/documents/data/data.xlsx
+++ b/documents/data/data.xlsx
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="34">
   <si>
     <t>TRACE</t>
   </si>
@@ -159,6 +159,15 @@
   </si>
   <si>
     <t>Implementation Comparison</t>
+  </si>
+  <si>
+    <t>BASE</t>
+  </si>
+  <si>
+    <t>Space Utilization</t>
+  </si>
+  <si>
+    <t>Performance</t>
   </si>
 </sst>
 </file>
@@ -221,8 +230,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -242,17 +255,21 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -322,7 +339,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$40:$A$42</c:f>
+              <c:f>Sheet1!$A$41:$A$43</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -339,7 +356,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$40:$F$42</c:f>
+              <c:f>Sheet1!$G$41:$G$43</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="3"/>
@@ -373,7 +390,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$40:$A$42</c:f>
+              <c:f>Sheet1!$A$41:$A$43</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -390,7 +407,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$40:$G$42</c:f>
+              <c:f>Sheet1!$H$41:$H$43</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="3"/>
@@ -433,7 +450,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$40:$A$42</c:f>
+              <c:f>Sheet1!$A$41:$A$43</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -450,7 +467,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$40:$H$42</c:f>
+              <c:f>Sheet1!$I$41:$I$43</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="3"/>
@@ -573,20 +590,385 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Normalized Compressed Cache Utilization for Benchmarks</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>BASELINE</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Sheet1!$A$19,Sheet1!$A$21,Sheet1!$A$25)</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>bisort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>llu</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$47:$F$49</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>POOLING</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Sheet1!$A$19,Sheet1!$A$21,Sheet1!$A$25)</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>bisort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>llu</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$47:$G$49</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.001573525434563</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.000383758970183</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.000180222535653</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>BASE-DELTA</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Sheet1!$A$19,Sheet1!$A$21,Sheet1!$A$25)</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>bisort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>llu</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$47:$H$49</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.996514797337325</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>BD+POOL</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="85000"/>
+                <a:lumOff val="15000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Sheet1!$A$19,Sheet1!$A$21,Sheet1!$A$25)</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>bisort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>llu</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$47:$I$49</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.001573525434563</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.995776462588607</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.000180222535653</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2140252056"/>
+        <c:axId val="2133755912"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2140252056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2133755912"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2133755912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.8"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Normalized Compressed</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Size</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2140252056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.255686872633287"/>
+          <c:y val="0.882057349783149"/>
+          <c:w val="0.448732718570606"/>
+          <c:h val="0.0645752841987999"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>317500</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -602,6 +984,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -943,10 +1357,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -957,7 +1371,7 @@
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="12.83203125" customWidth="1"/>
     <col min="6" max="6" width="12.1640625" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
     <col min="11" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
@@ -1681,7 +2095,7 @@
         <v>9.2591536871288738E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -1702,7 +2116,7 @@
         <v>0.45454545454545459</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
         <v>11</v>
       </c>
@@ -1723,7 +2137,7 @@
         <v>9.6153846153846145E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -1744,7 +2158,7 @@
         <v>0.45853658536585362</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
         <v>13</v>
       </c>
@@ -1765,143 +2179,314 @@
         <v>4.7808764940239001E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:9">
       <c r="A38" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F38" s="1" t="s">
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="3" t="s">
+    <row r="40" spans="1:9">
+      <c r="A40" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C40" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D40" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E40" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="F40" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G40" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G39" s="3" t="s">
+      <c r="H40" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H39" s="3" t="s">
+      <c r="I40" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
-      <c r="A40" t="s">
+    <row r="41" spans="1:9">
+      <c r="A41" t="s">
         <v>7</v>
       </c>
-      <c r="B40">
+      <c r="B41">
         <f>C8</f>
         <v>32</v>
       </c>
-      <c r="C40">
+      <c r="C41">
         <f>C7</f>
         <v>20</v>
       </c>
-      <c r="D40">
+      <c r="D41">
         <f>C19</f>
         <v>27.953099999999999</v>
       </c>
-      <c r="E40">
+      <c r="E41">
         <f>C18</f>
         <v>17.625</v>
       </c>
-      <c r="F40" s="2">
-        <f>C40/B40</f>
+      <c r="F41" s="2">
+        <f>B41/B41</f>
+        <v>1</v>
+      </c>
+      <c r="G41" s="2">
+        <f>C41/B41</f>
         <v>0.625</v>
       </c>
-      <c r="G40" s="2">
-        <f>D40/B40</f>
+      <c r="H41" s="2">
+        <f>D41/B41</f>
         <v>0.87353437499999997</v>
       </c>
-      <c r="H40" s="2">
-        <f>E40/B40</f>
+      <c r="I41" s="2">
+        <f>E41/B41</f>
         <v>0.55078125</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
-      <c r="A41" t="s">
+    <row r="42" spans="1:9">
+      <c r="A42" t="s">
         <v>9</v>
       </c>
-      <c r="B41">
+      <c r="B42">
         <f>C10</f>
         <v>66.656199999999998</v>
       </c>
-      <c r="C41">
+      <c r="C42">
         <f>C9</f>
         <v>50.218800000000002</v>
       </c>
-      <c r="D41">
+      <c r="D42">
         <f>C21</f>
         <v>60.484400000000001</v>
       </c>
-      <c r="E41">
+      <c r="E42">
         <f>C20</f>
         <v>17.8828</v>
       </c>
-      <c r="F41" s="2">
-        <f t="shared" ref="F41:F42" si="5">C41/B41</f>
+      <c r="F42" s="2">
+        <f t="shared" ref="F42:F43" si="5">B42/B42</f>
+        <v>1</v>
+      </c>
+      <c r="G42" s="2">
+        <f>C42/B42</f>
         <v>0.75340028384456359</v>
       </c>
-      <c r="G41" s="2">
-        <f t="shared" ref="G41:G42" si="6">D41/B41</f>
+      <c r="H42" s="2">
+        <f>D42/B42</f>
         <v>0.90740846312871126</v>
       </c>
-      <c r="H41" s="2">
-        <f t="shared" ref="H41:H42" si="7">E41/B41</f>
+      <c r="I42" s="2">
+        <f>E42/B42</f>
         <v>0.26828412060693529</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
-      <c r="A42" t="s">
+    <row r="43" spans="1:9">
+      <c r="A43" t="s">
         <v>13</v>
       </c>
-      <c r="B42">
+      <c r="B43">
         <f>C14</f>
         <v>7.84375</v>
       </c>
-      <c r="C42">
+      <c r="C43">
         <f>C13</f>
         <v>6.40625</v>
       </c>
-      <c r="D42">
+      <c r="D43">
         <f>C25</f>
         <v>7.46875</v>
       </c>
-      <c r="E42">
+      <c r="E43">
         <f>C24</f>
         <v>3.46875</v>
       </c>
-      <c r="F42" s="2">
+      <c r="F43" s="2">
         <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G43" s="2">
+        <f>C43/B43</f>
         <v>0.81673306772908372</v>
       </c>
-      <c r="G42" s="2">
+      <c r="H43" s="2">
+        <f>D43/B43</f>
+        <v>0.952191235059761</v>
+      </c>
+      <c r="I43" s="2">
+        <f>E43/B43</f>
+        <v>0.44223107569721115</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" s="2">
+        <f>H8</f>
+        <v>0.99582146558830009</v>
+      </c>
+      <c r="C47" s="2">
+        <f>H7</f>
+        <v>0.99738841599268757</v>
+      </c>
+      <c r="D47" s="2">
+        <f>H19</f>
+        <v>0.99582146558830009</v>
+      </c>
+      <c r="E47" s="2">
+        <f>H18</f>
+        <v>0.99738841599268757</v>
+      </c>
+      <c r="F47" s="2">
+        <f>B47/B47</f>
+        <v>1</v>
+      </c>
+      <c r="G47" s="2">
+        <f>C47/B47</f>
+        <v>1.0015735254345635</v>
+      </c>
+      <c r="H47" s="2">
+        <f>D47/B47</f>
+        <v>1</v>
+      </c>
+      <c r="I47" s="2">
+        <f>E47/B47</f>
+        <v>1.0015735254345635</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" t="s">
+        <v>9</v>
+      </c>
+      <c r="B48" s="2">
+        <f>H10</f>
+        <v>0.99844622428129681</v>
+      </c>
+      <c r="C48" s="2">
+        <f>H9</f>
+        <v>0.99882938697611057</v>
+      </c>
+      <c r="D48" s="2">
+        <f>H21</f>
+        <v>0.99496643684189434</v>
+      </c>
+      <c r="E48" s="2">
+        <f>H20</f>
+        <v>0.99422924929978107</v>
+      </c>
+      <c r="F48" s="2">
+        <f t="shared" ref="F48:F49" si="6">B48/B48</f>
+        <v>1</v>
+      </c>
+      <c r="G48" s="2">
+        <f t="shared" ref="G48:G49" si="7">C48/B48</f>
+        <v>1.0003837589701834</v>
+      </c>
+      <c r="H48" s="2">
+        <f t="shared" ref="H48:H49" si="8">D48/B48</f>
+        <v>0.99651479733732551</v>
+      </c>
+      <c r="I48" s="2">
+        <f t="shared" ref="I48:I49" si="9">E48/B48</f>
+        <v>0.99577646258860741</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49" s="2">
+        <f>H14</f>
+        <v>0.99901757791859591</v>
+      </c>
+      <c r="C49" s="2">
+        <f>H13</f>
+        <v>0.99919762339965013</v>
+      </c>
+      <c r="D49" s="2">
+        <f>H25</f>
+        <v>0.99901757791859591</v>
+      </c>
+      <c r="E49" s="2">
+        <f>H24</f>
+        <v>0.99919762339965013</v>
+      </c>
+      <c r="F49" s="2">
         <f t="shared" si="6"/>
-        <v>0.952191235059761</v>
-      </c>
-      <c r="H42" s="2">
+        <v>1</v>
+      </c>
+      <c r="G49" s="2">
         <f t="shared" si="7"/>
-        <v>0.44223107569721115</v>
+        <v>1.0001802225356529</v>
+      </c>
+      <c r="H49" s="2">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="I49" s="2">
+        <f t="shared" si="9"/>
+        <v>1.0001802225356529</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="73" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="95" fitToHeight="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="48" max="16383" man="1"/>
+  </rowBreaks>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>
@@ -1918,14 +2503,14 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="65" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
new chart template, and better labels
</commit_message>
<xml_diff>
--- a/documents/data/data.xlsx
+++ b/documents/data/data.xlsx
@@ -323,10 +323,10 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="2"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>POOLING</c:v>
+            <c:v>BASELINE</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -356,6 +356,40 @@
           </c:cat>
           <c:val>
             <c:numRef>
+              <c:f>Sheet1!$F$41:$F$43</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>POOLING</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
               <c:f>Sheet1!$G$41:$G$43</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
@@ -375,7 +409,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:v>BASE-DELTA</c:v>
           </c:tx>
@@ -388,23 +422,6 @@
             </a:solidFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$41:$A$43</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>bisort</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>llu</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>sort</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$H$41:$H$43</c:f>
@@ -425,8 +442,8 @@
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:idx val="3"/>
+          <c:order val="3"/>
           <c:tx>
             <c:v>BD+POOL</c:v>
           </c:tx>
@@ -448,23 +465,6 @@
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$41:$A$43</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>bisort</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>llu</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>sort</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$I$41:$I$43</c:f>
@@ -572,8 +572,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.255686872633287"/>
           <c:y val="0.882057349783149"/>
-          <c:w val="0.475267476107471"/>
-          <c:h val="0.0929872134967086"/>
+          <c:w val="0.448732718570606"/>
+          <c:h val="0.0645752841987999"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -617,7 +617,7 @@
               <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Normalized Compressed Cache Utilization for Benchmarks</a:t>
+              <a:t>Normalized Hit Ratios for Benchmarks</a:t>
             </a:r>
             <a:endParaRPr lang="en-US">
               <a:effectLst/>
@@ -648,6 +648,9 @@
                 <a:lumOff val="50000"/>
               </a:schemeClr>
             </a:solidFill>
+            <a:ln w="3175" cmpd="sng">
+              <a:noFill/>
+            </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -907,11 +910,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Normalized Compressed</a:t>
+                  <a:t>Normalized</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Size</a:t>
+                  <a:t> Hit Ratios for Benchmarks</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -2503,7 +2506,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
new graph for pooling effect
</commit_message>
<xml_diff>
--- a/documents/data/data.xlsx
+++ b/documents/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="38">
   <si>
     <t>TRACE</t>
   </si>
@@ -134,12 +134,6 @@
     <t>Base-Delta</t>
   </si>
   <si>
-    <t>Comparison</t>
-  </si>
-  <si>
-    <t>COMPRESSION</t>
-  </si>
-  <si>
     <t>Cache</t>
   </si>
   <si>
@@ -168,6 +162,24 @@
   </si>
   <si>
     <t>Performance</t>
+  </si>
+  <si>
+    <t>Effect of Pooling on Base-Delta</t>
+  </si>
+  <si>
+    <t>ZEROS</t>
+  </si>
+  <si>
+    <t>REPEATED</t>
+  </si>
+  <si>
+    <t>MEDIUM</t>
+  </si>
+  <si>
+    <t>LARGE</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -230,8 +242,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -255,7 +275,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -263,6 +283,10 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -270,6 +294,10 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -339,7 +367,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$41:$A$43</c:f>
+              <c:f>Sheet1!$A$30:$A$32</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -356,7 +384,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$41:$F$43</c:f>
+              <c:f>Sheet1!$F$30:$F$32</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="3"/>
@@ -390,7 +418,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$41:$G$43</c:f>
+              <c:f>Sheet1!$G$30:$G$32</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="3"/>
@@ -424,7 +452,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$41:$H$43</c:f>
+              <c:f>Sheet1!$H$30:$H$32</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="3"/>
@@ -449,10 +477,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="85000"/>
-                <a:lumOff val="15000"/>
-              </a:schemeClr>
+              <a:srgbClr val="008000"/>
             </a:solidFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
@@ -467,7 +492,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$41:$I$43</c:f>
+              <c:f>Sheet1!$I$30:$I$32</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="3"/>
@@ -582,6 +607,11 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -672,7 +702,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$47:$F$49</c:f>
+              <c:f>Sheet1!$F$36:$F$38</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="3"/>
@@ -723,7 +753,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$47:$G$49</c:f>
+              <c:f>Sheet1!$G$36:$G$38</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="3"/>
@@ -774,7 +804,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$47:$H$49</c:f>
+              <c:f>Sheet1!$H$36:$H$38</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="3"/>
@@ -834,7 +864,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$47:$I$49</c:f>
+              <c:f>Sheet1!$I$36:$I$38</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="3"/>
@@ -950,6 +980,506 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Effect of Pooling on Base-Delta Block Types</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="percentStacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>LARGE</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="85000"/>
+                <a:lumOff val="15000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$42:$A$47</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>bisort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bisort.pool</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>llu</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>llu.pool</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>sort</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>sort.pool</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$42:$E$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>767.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>488.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1763.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>251.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>MEDIUM</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$42:$A$47</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>bisort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bisort.pool</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>llu</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>llu.pool</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>sort</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>sort.pool</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$42:$D$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>253.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>152.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>345.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>624.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>REPEATED</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$42:$A$47</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>bisort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bisort.pool</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>llu</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>llu.pool</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>sort</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>sort.pool</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$42:$C$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>ZEROS</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="008000"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>53%</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>61%</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$42:$A$47</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>bisort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bisort.pool</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>llu</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>llu.pool</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>sort</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>sort.pool</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$42:$B$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>833.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>125.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="-2140504232"/>
+        <c:axId val="-2143412200"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2140504232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2143412200"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2143412200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Fraction of Blocks Used of Partoular Type</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2140504232"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.2"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.341248333263155"/>
+          <c:y val="0.898134541863939"/>
+          <c:w val="0.376226507782784"/>
+          <c:h val="0.0645752841987999"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -1019,6 +1549,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1360,10 +1922,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1374,8 +1936,7 @@
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="12.83203125" customWidth="1"/>
     <col min="6" max="6" width="12.1640625" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="7" max="8" width="12.6640625" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
     <col min="11" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.83203125" customWidth="1"/>
@@ -1386,7 +1947,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1994,501 +2555,483 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E28" s="3" t="s">
+      <c r="B29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29" s="2">
-        <f>G18-G7</f>
-        <v>-1.15966796875E-3</v>
-      </c>
-      <c r="C29" s="2">
-        <f>H18-H7</f>
-        <v>0</v>
-      </c>
-      <c r="D29" s="2">
-        <f>I18-I7</f>
-        <v>0</v>
-      </c>
-      <c r="E29" s="2">
-        <f>1-C18/C7</f>
-        <v>0.11875000000000002</v>
+      <c r="D29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="2">
-        <f>G19-G8</f>
-        <v>-1.9760253906250004E-3</v>
-      </c>
-      <c r="C30" s="2">
-        <f>H19-H8</f>
-        <v>0</v>
-      </c>
-      <c r="D30" s="2">
-        <f>I19-I8</f>
-        <v>0</v>
-      </c>
-      <c r="E30" s="2">
-        <f t="shared" ref="E30:E36" si="4">1-C19/C8</f>
-        <v>0.12646562500000003</v>
+      <c r="B30">
+        <f>C8</f>
+        <v>32</v>
+      </c>
+      <c r="C30">
+        <f>C7</f>
+        <v>20</v>
+      </c>
+      <c r="D30">
+        <f>C19</f>
+        <v>27.953099999999999</v>
+      </c>
+      <c r="E30">
+        <f>C18</f>
+        <v>17.625</v>
+      </c>
+      <c r="F30" s="2">
+        <f>B30/B30</f>
+        <v>1</v>
+      </c>
+      <c r="G30" s="2">
+        <f>C30/B30</f>
+        <v>0.625</v>
+      </c>
+      <c r="H30" s="2">
+        <f>D30/B30</f>
+        <v>0.87353437499999997</v>
+      </c>
+      <c r="I30" s="2">
+        <f>E30/B30</f>
+        <v>0.55078125</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>8</v>
-      </c>
-      <c r="B31" s="2">
-        <f>G20-G9</f>
-        <v>-1.5789062499999999E-2</v>
-      </c>
-      <c r="C31" s="2">
-        <f>H20-H9</f>
-        <v>-4.6001376763294965E-3</v>
-      </c>
-      <c r="D31" s="2">
-        <f>I20-I9</f>
-        <v>4.6001376763295052E-3</v>
-      </c>
-      <c r="E31" s="2">
-        <f t="shared" si="4"/>
-        <v>0.64390228360693613</v>
+        <v>9</v>
+      </c>
+      <c r="B31">
+        <f>C10</f>
+        <v>66.656199999999998</v>
+      </c>
+      <c r="C31">
+        <f>C9</f>
+        <v>50.218800000000002</v>
+      </c>
+      <c r="D31">
+        <f>C21</f>
+        <v>60.484400000000001</v>
+      </c>
+      <c r="E31">
+        <f>C20</f>
+        <v>17.8828</v>
+      </c>
+      <c r="F31" s="2">
+        <f t="shared" ref="F31:F32" si="4">B31/B31</f>
+        <v>1</v>
+      </c>
+      <c r="G31" s="2">
+        <f>C31/B31</f>
+        <v>0.75340028384456359</v>
+      </c>
+      <c r="H31" s="2">
+        <f>D31/B31</f>
+        <v>0.90740846312871126</v>
+      </c>
+      <c r="I31" s="2">
+        <f>E31/B31</f>
+        <v>0.26828412060693529</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>9</v>
-      </c>
-      <c r="B32" s="2">
-        <f>G21-G10</f>
-        <v>-3.0135742187499988E-3</v>
-      </c>
-      <c r="C32" s="2">
-        <f>H21-H10</f>
-        <v>-3.4797874394024708E-3</v>
-      </c>
-      <c r="D32" s="2">
-        <f>I21-I10</f>
-        <v>3.4797874394023828E-3</v>
-      </c>
-      <c r="E32" s="2">
-        <f t="shared" si="4"/>
-        <v>9.2591536871288738E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" t="s">
-        <v>10</v>
-      </c>
-      <c r="B33" s="2">
-        <f>G22-G11</f>
-        <v>-3.0517578125E-4</v>
-      </c>
-      <c r="C33" s="2">
-        <f>H22-H11</f>
-        <v>0</v>
-      </c>
-      <c r="D33" s="2">
-        <f>I22-I11</f>
-        <v>0</v>
-      </c>
-      <c r="E33" s="2">
-        <f t="shared" si="4"/>
-        <v>0.45454545454545459</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" t="s">
-        <v>11</v>
-      </c>
-      <c r="B34" s="2">
-        <f>G23-G12</f>
-        <v>-7.62939453125E-5</v>
-      </c>
-      <c r="C34" s="2">
-        <f>H23-H12</f>
-        <v>0</v>
-      </c>
-      <c r="D34" s="2">
-        <f>I23-I12</f>
-        <v>0</v>
-      </c>
-      <c r="E34" s="2">
-        <f t="shared" si="4"/>
-        <v>9.6153846153846145E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" t="s">
-        <v>12</v>
-      </c>
-      <c r="B35" s="2">
-        <f>G24-G13</f>
-        <v>-1.434326171875E-3</v>
-      </c>
-      <c r="C35" s="2">
-        <f>H24-H13</f>
-        <v>0</v>
-      </c>
-      <c r="D35" s="2">
-        <f>I24-I13</f>
-        <v>0</v>
-      </c>
-      <c r="E35" s="2">
-        <f t="shared" si="4"/>
-        <v>0.45853658536585362</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" t="s">
         <v>13</v>
       </c>
-      <c r="B36" s="2">
-        <f>G25-G14</f>
-        <v>-1.8310546875E-4</v>
-      </c>
-      <c r="C36" s="2">
-        <f>H25-H14</f>
-        <v>0</v>
-      </c>
-      <c r="D36" s="2">
-        <f>I25-I14</f>
-        <v>0</v>
-      </c>
-      <c r="E36" s="2">
-        <f t="shared" si="4"/>
-        <v>4.7808764940239001E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I40" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" t="s">
-        <v>7</v>
-      </c>
-      <c r="B41">
-        <f>C8</f>
-        <v>32</v>
-      </c>
-      <c r="C41">
-        <f>C7</f>
-        <v>20</v>
-      </c>
-      <c r="D41">
-        <f>C19</f>
-        <v>27.953099999999999</v>
-      </c>
-      <c r="E41">
-        <f>C18</f>
-        <v>17.625</v>
-      </c>
-      <c r="F41" s="2">
-        <f>B41/B41</f>
-        <v>1</v>
-      </c>
-      <c r="G41" s="2">
-        <f>C41/B41</f>
-        <v>0.625</v>
-      </c>
-      <c r="H41" s="2">
-        <f>D41/B41</f>
-        <v>0.87353437499999997</v>
-      </c>
-      <c r="I41" s="2">
-        <f>E41/B41</f>
-        <v>0.55078125</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" t="s">
-        <v>9</v>
-      </c>
-      <c r="B42">
-        <f>C10</f>
-        <v>66.656199999999998</v>
-      </c>
-      <c r="C42">
-        <f>C9</f>
-        <v>50.218800000000002</v>
-      </c>
-      <c r="D42">
-        <f>C21</f>
-        <v>60.484400000000001</v>
-      </c>
-      <c r="E42">
-        <f>C20</f>
-        <v>17.8828</v>
-      </c>
-      <c r="F42" s="2">
-        <f t="shared" ref="F42:F43" si="5">B42/B42</f>
-        <v>1</v>
-      </c>
-      <c r="G42" s="2">
-        <f>C42/B42</f>
-        <v>0.75340028384456359</v>
-      </c>
-      <c r="H42" s="2">
-        <f>D42/B42</f>
-        <v>0.90740846312871126</v>
-      </c>
-      <c r="I42" s="2">
-        <f>E42/B42</f>
-        <v>0.26828412060693529</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43" t="s">
-        <v>13</v>
-      </c>
-      <c r="B43">
+      <c r="B32">
         <f>C14</f>
         <v>7.84375</v>
       </c>
-      <c r="C43">
+      <c r="C32">
         <f>C13</f>
         <v>6.40625</v>
       </c>
-      <c r="D43">
+      <c r="D32">
         <f>C25</f>
         <v>7.46875</v>
       </c>
-      <c r="E43">
+      <c r="E32">
         <f>C24</f>
         <v>3.46875</v>
       </c>
-      <c r="F43" s="2">
+      <c r="F32" s="2">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G32" s="2">
+        <f>C32/B32</f>
+        <v>0.81673306772908372</v>
+      </c>
+      <c r="H32" s="2">
+        <f>D32/B32</f>
+        <v>0.952191235059761</v>
+      </c>
+      <c r="I32" s="2">
+        <f>E32/B32</f>
+        <v>0.44223107569721115</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="2">
+        <f>H8</f>
+        <v>0.99582146558830009</v>
+      </c>
+      <c r="C36" s="2">
+        <f>H7</f>
+        <v>0.99738841599268757</v>
+      </c>
+      <c r="D36" s="2">
+        <f>H19</f>
+        <v>0.99582146558830009</v>
+      </c>
+      <c r="E36" s="2">
+        <f>H18</f>
+        <v>0.99738841599268757</v>
+      </c>
+      <c r="F36" s="2">
+        <f>B36/B36</f>
+        <v>1</v>
+      </c>
+      <c r="G36" s="2">
+        <f>C36/B36</f>
+        <v>1.0015735254345635</v>
+      </c>
+      <c r="H36" s="2">
+        <f>D36/B36</f>
+        <v>1</v>
+      </c>
+      <c r="I36" s="2">
+        <f>E36/B36</f>
+        <v>1.0015735254345635</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="2">
+        <f>H10</f>
+        <v>0.99844622428129681</v>
+      </c>
+      <c r="C37" s="2">
+        <f>H9</f>
+        <v>0.99882938697611057</v>
+      </c>
+      <c r="D37" s="2">
+        <f>H21</f>
+        <v>0.99496643684189434</v>
+      </c>
+      <c r="E37" s="2">
+        <f>H20</f>
+        <v>0.99422924929978107</v>
+      </c>
+      <c r="F37" s="2">
+        <f t="shared" ref="F37:F38" si="5">B37/B37</f>
+        <v>1</v>
+      </c>
+      <c r="G37" s="2">
+        <f t="shared" ref="G37:G38" si="6">C37/B37</f>
+        <v>1.0003837589701834</v>
+      </c>
+      <c r="H37" s="2">
+        <f t="shared" ref="H37:H38" si="7">D37/B37</f>
+        <v>0.99651479733732551</v>
+      </c>
+      <c r="I37" s="2">
+        <f t="shared" ref="I37:I38" si="8">E37/B37</f>
+        <v>0.99577646258860741</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" s="2">
+        <f>H14</f>
+        <v>0.99901757791859591</v>
+      </c>
+      <c r="C38" s="2">
+        <f>H13</f>
+        <v>0.99919762339965013</v>
+      </c>
+      <c r="D38" s="2">
+        <f>H25</f>
+        <v>0.99901757791859591</v>
+      </c>
+      <c r="E38" s="2">
+        <f>H24</f>
+        <v>0.99919762339965013</v>
+      </c>
+      <c r="F38" s="2">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="G43" s="2">
-        <f>C43/B43</f>
-        <v>0.81673306772908372</v>
-      </c>
-      <c r="H43" s="2">
-        <f>D43/B43</f>
-        <v>0.952191235059761</v>
-      </c>
-      <c r="I43" s="2">
-        <f>E43/B43</f>
-        <v>0.44223107569721115</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="1" t="s">
+      <c r="G38" s="2">
+        <f t="shared" si="6"/>
+        <v>1.0001802225356529</v>
+      </c>
+      <c r="H38" s="2">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" si="8"/>
+        <v>1.0001802225356529</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="3" t="s">
+      <c r="C41" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42">
+        <v>4</v>
+      </c>
+      <c r="C42">
         <v>0</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="D42">
+        <v>253</v>
+      </c>
+      <c r="E42">
+        <v>767</v>
+      </c>
+      <c r="F42">
+        <f>SUM(B42:E42)</f>
+        <v>1024</v>
+      </c>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>152</v>
+      </c>
+      <c r="E43">
+        <v>488</v>
+      </c>
+      <c r="F43">
+        <f>SUM(B43:E43)</f>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>345</v>
+      </c>
+      <c r="E44">
+        <v>1763</v>
+      </c>
+      <c r="F44">
+        <f>SUM(B44:E44)</f>
+        <v>2108</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45">
+        <v>833</v>
+      </c>
+      <c r="C45">
+        <v>97</v>
+      </c>
+      <c r="D45">
+        <v>624</v>
+      </c>
+      <c r="E45">
         <v>28</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I46" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
+      <c r="F45">
+        <f>SUM(B45:E45)</f>
+        <v>1582</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>251</v>
+      </c>
+      <c r="F46">
+        <f>SUM(B46:E46)</f>
+        <v>251</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
       <c r="A47" t="s">
-        <v>7</v>
-      </c>
-      <c r="B47" s="2">
-        <f>H8</f>
-        <v>0.99582146558830009</v>
-      </c>
-      <c r="C47" s="2">
-        <f>H7</f>
-        <v>0.99738841599268757</v>
-      </c>
-      <c r="D47" s="2">
-        <f>H19</f>
-        <v>0.99582146558830009</v>
-      </c>
-      <c r="E47" s="2">
-        <f>H18</f>
-        <v>0.99738841599268757</v>
-      </c>
-      <c r="F47" s="2">
-        <f>B47/B47</f>
-        <v>1</v>
-      </c>
-      <c r="G47" s="2">
-        <f>C47/B47</f>
-        <v>1.0015735254345635</v>
-      </c>
-      <c r="H47" s="2">
-        <f>D47/B47</f>
-        <v>1</v>
-      </c>
-      <c r="I47" s="2">
-        <f>E47/B47</f>
-        <v>1.0015735254345635</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
-      <c r="A48" t="s">
-        <v>9</v>
-      </c>
-      <c r="B48" s="2">
-        <f>H10</f>
-        <v>0.99844622428129681</v>
-      </c>
-      <c r="C48" s="2">
-        <f>H9</f>
-        <v>0.99882938697611057</v>
-      </c>
-      <c r="D48" s="2">
-        <f>H21</f>
-        <v>0.99496643684189434</v>
-      </c>
-      <c r="E48" s="2">
-        <f>H20</f>
-        <v>0.99422924929978107</v>
-      </c>
-      <c r="F48" s="2">
-        <f t="shared" ref="F48:F49" si="6">B48/B48</f>
-        <v>1</v>
-      </c>
-      <c r="G48" s="2">
-        <f t="shared" ref="G48:G49" si="7">C48/B48</f>
-        <v>1.0003837589701834</v>
-      </c>
-      <c r="H48" s="2">
-        <f t="shared" ref="H48:H49" si="8">D48/B48</f>
-        <v>0.99651479733732551</v>
-      </c>
-      <c r="I48" s="2">
-        <f t="shared" ref="I48:I49" si="9">E48/B48</f>
-        <v>0.99577646258860741</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
-      <c r="A49" t="s">
-        <v>13</v>
-      </c>
-      <c r="B49" s="2">
-        <f>H14</f>
-        <v>0.99901757791859591</v>
-      </c>
-      <c r="C49" s="2">
-        <f>H13</f>
-        <v>0.99919762339965013</v>
-      </c>
-      <c r="D49" s="2">
-        <f>H25</f>
-        <v>0.99901757791859591</v>
-      </c>
-      <c r="E49" s="2">
-        <f>H24</f>
-        <v>0.99919762339965013</v>
-      </c>
-      <c r="F49" s="2">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="G49" s="2">
-        <f t="shared" si="7"/>
-        <v>1.0001802225356529</v>
-      </c>
-      <c r="H49" s="2">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="I49" s="2">
-        <f t="shared" si="9"/>
-        <v>1.0001802225356529</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B47">
+        <v>125</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>80</v>
+      </c>
+      <c r="F47">
+        <f>SUM(B47:E47)</f>
+        <v>205</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" s="1"/>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="95" fitToHeight="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0" footer="0"/>
+  <pageSetup scale="80" fitToHeight="0" pageOrder="overThenDown" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="48" max="16383" man="1"/>
+    <brk id="50" max="16383" man="1"/>
   </rowBreaks>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -2505,15 +3048,15 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="65" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="68" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
graph for compression ratios
</commit_message>
<xml_diff>
--- a/documents/data/data.xlsx
+++ b/documents/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="40">
   <si>
     <t>TRACE</t>
   </si>
@@ -180,6 +180,12 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Normalized Compression Ratio</t>
+  </si>
+  <si>
+    <t>Compressio Ratio</t>
   </si>
 </sst>
 </file>
@@ -242,7 +248,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -266,16 +272,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -287,6 +296,7 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -298,6 +308,7 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -332,7 +343,7 @@
               <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Normalized Compressed Cache Utilization for Benchmarks</a:t>
+              <a:t>Normalized Compression Ratio for Benchmarks</a:t>
             </a:r>
             <a:endParaRPr lang="en-US">
               <a:effectLst/>
@@ -384,9 +395,9 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$30:$F$32</c:f>
+              <c:f>Sheet1!$F$34:$F$36</c:f>
               <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
@@ -418,18 +429,18 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$30:$G$32</c:f>
+              <c:f>Sheet1!$G$34:$G$36</c:f>
               <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.625</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.753400283844564</c:v>
+                  <c:v>1.327315666642771</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.816733067729084</c:v>
+                  <c:v>1.224390243902439</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -452,18 +463,18 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$30:$H$32</c:f>
+              <c:f>Sheet1!$H$34:$H$36</c:f>
               <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.873534375</c:v>
+                  <c:v>1.144774640379779</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.907408463128711</c:v>
+                  <c:v>1.102039534160874</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.952191235059761</c:v>
+                  <c:v>1.05020920502092</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -492,18 +503,18 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$30:$I$32</c:f>
+              <c:f>Sheet1!$I$34:$I$36</c:f>
               <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.55078125</c:v>
+                  <c:v>1.815602836879433</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.268284120606935</c:v>
+                  <c:v>3.727391683628962</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.442231075697211</c:v>
+                  <c:v>2.261261261261261</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -518,11 +529,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2140568616"/>
-        <c:axId val="-2140838680"/>
+        <c:axId val="-2147010984"/>
+        <c:axId val="-2147007928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2140568616"/>
+        <c:axId val="-2147010984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -531,7 +542,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2140838680"/>
+        <c:crossAx val="-2147007928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -539,7 +550,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2140838680"/>
+        <c:axId val="-2147007928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -567,13 +578,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Normalized Compressed</a:t>
+                  <a:t>Normalized Compression Ratio</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Size</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -584,7 +590,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2140568616"/>
+        <c:crossAx val="-2147010984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -647,379 +653,6 @@
               <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Normalized Hit Ratios for Benchmarks</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US">
-              <a:effectLst/>
-            </a:endParaRPr>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>BASELINE</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="50000"/>
-                <a:lumOff val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln w="3175" cmpd="sng">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>(Sheet1!$A$19,Sheet1!$A$21,Sheet1!$A$25)</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>bisort</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>llu</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>sort</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$F$36:$F$38</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>POOLING</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="65000"/>
-                <a:lumOff val="35000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>(Sheet1!$A$19,Sheet1!$A$21,Sheet1!$A$25)</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>bisort</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>llu</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>sort</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$G$36:$G$38</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1.001573525434563</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.000383758970183</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.000180222535653</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>BASE-DELTA</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="75000"/>
-                <a:lumOff val="25000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>(Sheet1!$A$19,Sheet1!$A$21,Sheet1!$A$25)</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>bisort</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>llu</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>sort</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$H$36:$H$38</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.996514797337325</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>BD+POOL</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="85000"/>
-                <a:lumOff val="15000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>(Sheet1!$A$19,Sheet1!$A$21,Sheet1!$A$25)</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>bisort</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>llu</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>sort</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$I$36:$I$38</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1.001573525434563</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.995776462588607</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.000180222535653</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="-2140252056"/>
-        <c:axId val="2133755912"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="-2140252056"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2133755912"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2133755912"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="0.8"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Normalized</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Hit Ratios for Benchmarks</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2140252056"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.255686872633287"/>
-          <c:y val="0.882057349783149"/>
-          <c:w val="0.448732718570606"/>
-          <c:h val="0.0645752841987999"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
               <a:t>Effect of Pooling on Base-Delta Block Types</a:t>
             </a:r>
             <a:endParaRPr lang="en-US">
@@ -1055,7 +688,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$42:$A$47</c:f>
+              <c:f>Sheet1!$A$47:$A$52</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1081,7 +714,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$42:$E$47</c:f>
+              <c:f>Sheet1!$E$47:$E$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1124,7 +757,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$42:$A$47</c:f>
+              <c:f>Sheet1!$A$47:$A$52</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1150,7 +783,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$42:$D$47</c:f>
+              <c:f>Sheet1!$D$47:$D$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1193,7 +826,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$42:$A$47</c:f>
+              <c:f>Sheet1!$A$47:$A$52</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1219,7 +852,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$42:$C$47</c:f>
+              <c:f>Sheet1!$C$47:$C$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1328,7 +961,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$42:$A$47</c:f>
+              <c:f>Sheet1!$A$47:$A$52</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1354,7 +987,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$42:$B$47</c:f>
+              <c:f>Sheet1!$B$47:$B$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1390,11 +1023,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2140504232"/>
-        <c:axId val="-2143412200"/>
+        <c:axId val="-2130333688"/>
+        <c:axId val="-2128447224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2140504232"/>
+        <c:axId val="-2130333688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1403,7 +1036,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143412200"/>
+        <c:crossAx val="-2128447224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1411,7 +1044,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2143412200"/>
+        <c:axId val="-2128447224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1451,7 +1084,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2140504232"/>
+        <c:crossAx val="-2130333688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -1488,24 +1121,712 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Normalized Hit Ratios for Benchmarks</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>BASELINE</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="3175" cmpd="sng">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Sheet1!$A$19,Sheet1!$A$21,Sheet1!$A$25)</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>bisort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>llu</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$41:$F$43</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>POOLING</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Sheet1!$A$19,Sheet1!$A$21,Sheet1!$A$25)</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>bisort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>llu</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$41:$G$43</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.001573525434563</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.000383758970183</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.000180222535653</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>BASE-DELTA</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Sheet1!$A$19,Sheet1!$A$21,Sheet1!$A$25)</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>bisort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>llu</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$41:$H$43</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.996514797337325</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>BD+POOL</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="85000"/>
+                <a:lumOff val="15000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Sheet1!$A$19,Sheet1!$A$21,Sheet1!$A$25)</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>bisort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>llu</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$41:$I$43</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.001573525434563</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.995776462588607</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.000180222535653</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2124892360"/>
+        <c:axId val="-2125441800"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2124892360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2125441800"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2125441800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.8"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Normalized</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Hit Ratios for Benchmarks</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2124892360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.255686872633287"/>
+          <c:y val="0.882057349783149"/>
+          <c:w val="0.448732718570606"/>
+          <c:h val="0.0645752841987999"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Normalized Compressed Cache Utilization for Benchmarks</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>BASELINE</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$30:$A$32</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>bisort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>llu</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$30:$F$32</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>POOLING</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$30:$G$32</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.753400283844564</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.816733067729084</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>BASE-DELTA</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$30:$H$32</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.873534375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.907408463128711</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.952191235059761</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>BD+POOL</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="008000"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$30:$I$32</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.55078125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.268284120606935</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.442231075697211</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2142774472"/>
+        <c:axId val="-2126332264"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2142774472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2126332264"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2126332264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Normalized Compressed</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Size</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2142774472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.255686872633287"/>
+          <c:y val="0.882057349783149"/>
+          <c:w val="0.448732718570606"/>
+          <c:h val="0.0645752841987999"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -1524,20 +1845,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="7" name="Chart 6"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -1556,20 +1877,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="9" name="Chart 8"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -1581,6 +1902,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1922,10 +2275,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2706,333 +3059,389 @@
         <v>0.44223107569721115</v>
       </c>
     </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="34" spans="1:11">
-      <c r="A34" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>27</v>
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" s="4">
+        <f>1/F30</f>
+        <v>1</v>
+      </c>
+      <c r="G34" s="4">
+        <f>1/G30</f>
+        <v>1.6</v>
+      </c>
+      <c r="H34" s="4">
+        <f>1/H30</f>
+        <v>1.1447746403797789</v>
+      </c>
+      <c r="I34" s="4">
+        <f>1/I30</f>
+        <v>1.8156028368794326</v>
       </c>
     </row>
     <row r="35" spans="1:11">
-      <c r="A35" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>25</v>
+      <c r="A35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="4">
+        <f t="shared" ref="F35:F36" si="5">1/F31</f>
+        <v>1</v>
+      </c>
+      <c r="G35" s="4">
+        <f>1/G31</f>
+        <v>1.3273156666427712</v>
+      </c>
+      <c r="H35" s="4">
+        <f t="shared" ref="H35:I36" si="6">1/H31</f>
+        <v>1.1020395341608744</v>
+      </c>
+      <c r="I35" s="4">
+        <f t="shared" si="6"/>
+        <v>3.7273916836289618</v>
       </c>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G36" s="4">
+        <f>1/G32</f>
+        <v>1.224390243902439</v>
+      </c>
+      <c r="H36" s="4">
+        <f t="shared" si="6"/>
+        <v>1.0502092050209204</v>
+      </c>
+      <c r="I36" s="4">
+        <f t="shared" si="6"/>
+        <v>2.2612612612612613</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B41" s="2">
         <f>H8</f>
         <v>0.99582146558830009</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C41" s="2">
         <f>H7</f>
         <v>0.99738841599268757</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D41" s="2">
         <f>H19</f>
         <v>0.99582146558830009</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E41" s="2">
         <f>H18</f>
         <v>0.99738841599268757</v>
       </c>
-      <c r="F36" s="2">
-        <f>B36/B36</f>
+      <c r="F41" s="2">
+        <f>B41/B41</f>
         <v>1</v>
       </c>
-      <c r="G36" s="2">
-        <f>C36/B36</f>
+      <c r="G41" s="2">
+        <f>C41/B41</f>
         <v>1.0015735254345635</v>
       </c>
-      <c r="H36" s="2">
-        <f>D36/B36</f>
+      <c r="H41" s="2">
+        <f>D41/B41</f>
         <v>1</v>
       </c>
-      <c r="I36" s="2">
-        <f>E36/B36</f>
+      <c r="I41" s="2">
+        <f>E41/B41</f>
         <v>1.0015735254345635</v>
       </c>
-    </row>
-    <row r="37" spans="1:11">
-      <c r="A37" t="s">
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B42" s="2">
         <f>H10</f>
         <v>0.99844622428129681</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C42" s="2">
         <f>H9</f>
         <v>0.99882938697611057</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D42" s="2">
         <f>H21</f>
         <v>0.99496643684189434</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E42" s="2">
         <f>H20</f>
         <v>0.99422924929978107</v>
       </c>
-      <c r="F37" s="2">
-        <f t="shared" ref="F37:F38" si="5">B37/B37</f>
+      <c r="F42" s="2">
+        <f t="shared" ref="F42:F43" si="7">B42/B42</f>
         <v>1</v>
       </c>
-      <c r="G37" s="2">
-        <f t="shared" ref="G37:G38" si="6">C37/B37</f>
+      <c r="G42" s="2">
+        <f t="shared" ref="G42:G43" si="8">C42/B42</f>
         <v>1.0003837589701834</v>
       </c>
-      <c r="H37" s="2">
-        <f t="shared" ref="H37:H38" si="7">D37/B37</f>
+      <c r="H42" s="2">
+        <f t="shared" ref="H42:H43" si="9">D42/B42</f>
         <v>0.99651479733732551</v>
       </c>
-      <c r="I37" s="2">
-        <f t="shared" ref="I37:I38" si="8">E37/B37</f>
+      <c r="I42" s="2">
+        <f t="shared" ref="I42:I43" si="10">E42/B42</f>
         <v>0.99577646258860741</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
-      <c r="A38" t="s">
+    <row r="43" spans="1:11">
+      <c r="A43" t="s">
         <v>13</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B43" s="2">
         <f>H14</f>
         <v>0.99901757791859591</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C43" s="2">
         <f>H13</f>
         <v>0.99919762339965013</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D43" s="2">
         <f>H25</f>
         <v>0.99901757791859591</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E43" s="2">
         <f>H24</f>
         <v>0.99919762339965013</v>
       </c>
-      <c r="F38" s="2">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="G38" s="2">
-        <f t="shared" si="6"/>
-        <v>1.0001802225356529</v>
-      </c>
-      <c r="H38" s="2">
+      <c r="F43" s="2">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="I38" s="2">
+      <c r="G43" s="2">
         <f t="shared" si="8"/>
         <v>1.0001802225356529</v>
       </c>
-    </row>
-    <row r="40" spans="1:11">
-      <c r="A40" s="1" t="s">
+      <c r="H43" s="2">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="I43" s="2">
+        <f t="shared" si="10"/>
+        <v>1.0001802225356529</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="1:11">
-      <c r="A41" s="3" t="s">
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B46" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C46" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D46" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E46" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="F46" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-    </row>
-    <row r="42" spans="1:11">
-      <c r="A42" t="s">
-        <v>7</v>
-      </c>
-      <c r="B42">
-        <v>4</v>
-      </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
-      <c r="D42">
-        <v>253</v>
-      </c>
-      <c r="E42">
-        <v>767</v>
-      </c>
-      <c r="F42">
-        <f>SUM(B42:E42)</f>
-        <v>1024</v>
-      </c>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-    </row>
-    <row r="43" spans="1:11">
-      <c r="A43" t="s">
-        <v>6</v>
-      </c>
-      <c r="B43">
-        <v>0</v>
-      </c>
-      <c r="C43">
-        <v>0</v>
-      </c>
-      <c r="D43">
-        <v>152</v>
-      </c>
-      <c r="E43">
-        <v>488</v>
-      </c>
-      <c r="F43">
-        <f>SUM(B43:E43)</f>
-        <v>640</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11">
-      <c r="A44" t="s">
-        <v>9</v>
-      </c>
-      <c r="B44">
-        <v>0</v>
-      </c>
-      <c r="C44">
-        <v>0</v>
-      </c>
-      <c r="D44">
-        <v>345</v>
-      </c>
-      <c r="E44">
-        <v>1763</v>
-      </c>
-      <c r="F44">
-        <f>SUM(B44:E44)</f>
-        <v>2108</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11">
-      <c r="A45" t="s">
-        <v>8</v>
-      </c>
-      <c r="B45">
-        <v>833</v>
-      </c>
-      <c r="C45">
-        <v>97</v>
-      </c>
-      <c r="D45">
-        <v>624</v>
-      </c>
-      <c r="E45">
-        <v>28</v>
-      </c>
-      <c r="F45">
-        <f>SUM(B45:E45)</f>
-        <v>1582</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11">
-      <c r="A46" t="s">
-        <v>13</v>
-      </c>
-      <c r="B46">
-        <v>0</v>
-      </c>
-      <c r="C46">
-        <v>0</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46">
-        <v>251</v>
-      </c>
-      <c r="F46">
-        <f>SUM(B46:E46)</f>
-        <v>251</v>
-      </c>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
     </row>
     <row r="47" spans="1:11">
       <c r="A47" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B47">
-        <v>125</v>
+        <v>4</v>
       </c>
       <c r="C47">
         <v>0</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>253</v>
       </c>
       <c r="E47">
-        <v>80</v>
+        <v>767</v>
       </c>
       <c r="F47">
         <f>SUM(B47:E47)</f>
+        <v>1024</v>
+      </c>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>152</v>
+      </c>
+      <c r="E48">
+        <v>488</v>
+      </c>
+      <c r="F48">
+        <f>SUM(B48:E48)</f>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>345</v>
+      </c>
+      <c r="E49">
+        <v>1763</v>
+      </c>
+      <c r="F49">
+        <f>SUM(B49:E49)</f>
+        <v>2108</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50">
+        <v>833</v>
+      </c>
+      <c r="C50">
+        <v>97</v>
+      </c>
+      <c r="D50">
+        <v>624</v>
+      </c>
+      <c r="E50">
+        <v>28</v>
+      </c>
+      <c r="F50">
+        <f>SUM(B50:E50)</f>
+        <v>1582</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>13</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>251</v>
+      </c>
+      <c r="F51">
+        <f>SUM(B51:E51)</f>
+        <v>251</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52">
+        <v>125</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>80</v>
+      </c>
+      <c r="F52">
+        <f>SUM(B52:E52)</f>
         <v>205</v>
       </c>
-    </row>
-    <row r="48" spans="1:11">
-      <c r="A48" s="1"/>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0" footer="0"/>
   <pageSetup scale="80" fitToHeight="0" pageOrder="overThenDown" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <rowBreaks count="1" manualBreakCount="1">
-    <brk id="50" max="16383" man="1"/>
-  </rowBreaks>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>
@@ -3048,8 +3457,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="L45" sqref="L45"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
added meaning less hit ratio data and poster
</commit_message>
<xml_diff>
--- a/documents/data/data.xlsx
+++ b/documents/data/data.xlsx
@@ -1330,10 +1330,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="85000"/>
-                <a:lumOff val="15000"/>
-              </a:schemeClr>
+              <a:srgbClr val="008000"/>
             </a:solidFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
@@ -3457,8 +3454,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
test traces, bisort data, gitignore
</commit_message>
<xml_diff>
--- a/documents/data/data.xlsx
+++ b/documents/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1180" yWindow="200" windowWidth="25300" windowHeight="17000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,8 +14,9 @@
     <definedName name="results" localSheetId="0">Sheet1!#REF!</definedName>
     <definedName name="results_1" localSheetId="0">Sheet1!$A$5:$F$25</definedName>
     <definedName name="results_2" localSheetId="0">Sheet1!$K$9:$P$30</definedName>
+    <definedName name="results_3" localSheetId="0">Sheet1!$L$6:$Q$21</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,8 +27,8 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="results.csv" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="data:documents:cmu ece comp research:shared:data:results.csv" comma="1">
+  <connection id="1" name="results.csv1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="data:documents:cmu ece comp research:shared:data:results.csv" comma="1">
       <textFields count="6">
         <textField/>
         <textField/>
@@ -38,8 +39,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="results.csv1" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="data:documents:cmu ece comp research:shared:data:results.csv" comma="1">
+  <connection id="2" name="results.csv2" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="data:documents:cmu ece comp research:shared:data:results.csv" comma="1">
       <textFields count="6">
         <textField/>
         <textField/>
@@ -50,8 +51,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="results.csv2" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="data:documents:cmu ece comp research:shared:data:results.csv" comma="1">
+  <connection id="3" name="results.csv3" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="data:documents:cmu ece comp research:shared:data:results.csv" comma="1">
       <textFields count="6">
         <textField/>
         <textField/>
@@ -248,8 +249,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -284,7 +289,7 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -297,6 +302,8 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -309,6 +316,8 @@
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -471,7 +480,7 @@
                   <c:v>1.144774640379779</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.102039534160874</c:v>
+                  <c:v>1.017409594050882</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.05020920502092</c:v>
@@ -529,11 +538,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2147010984"/>
-        <c:axId val="-2147007928"/>
+        <c:axId val="-2143065544"/>
+        <c:axId val="-2140767272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2147010984"/>
+        <c:axId val="-2143065544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -542,7 +551,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2147007928"/>
+        <c:crossAx val="-2140767272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -550,7 +559,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2147007928"/>
+        <c:axId val="-2140767272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -590,7 +599,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2147010984"/>
+        <c:crossAx val="-2143065544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1023,11 +1032,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2130333688"/>
-        <c:axId val="-2128447224"/>
+        <c:axId val="2046924776"/>
+        <c:axId val="2046927880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2130333688"/>
+        <c:axId val="2046924776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1036,7 +1045,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2128447224"/>
+        <c:crossAx val="2046927880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1044,7 +1053,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2128447224"/>
+        <c:axId val="2046927880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1084,7 +1093,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130333688"/>
+        <c:crossAx val="2046924776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -1388,11 +1397,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2124892360"/>
-        <c:axId val="-2125441800"/>
+        <c:axId val="-2124233944"/>
+        <c:axId val="-2124230888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2124892360"/>
+        <c:axId val="-2124233944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1401,7 +1410,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2125441800"/>
+        <c:crossAx val="-2124230888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1409,7 +1418,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2125441800"/>
+        <c:axId val="-2124230888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.8"/>
@@ -1455,7 +1464,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124892360"/>
+        <c:crossAx val="-2124233944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1646,7 +1655,7 @@
                   <c:v>0.873534375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.907408463128711</c:v>
+                  <c:v>0.982888313465214</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.952191235059761</c:v>
@@ -1704,11 +1713,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2142774472"/>
-        <c:axId val="-2126332264"/>
+        <c:axId val="2037712680"/>
+        <c:axId val="-2123346600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2142774472"/>
+        <c:axId val="2037712680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1717,7 +1726,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2126332264"/>
+        <c:crossAx val="-2123346600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1725,7 +1734,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2126332264"/>
+        <c:axId val="-2123346600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1770,7 +1779,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2142774472"/>
+        <c:crossAx val="2037712680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1940,11 +1949,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results_2" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results_1" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results_1" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results_2" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results_3" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2274,8 +2287,8 @@
   </sheetPr>
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2289,10 +2302,12 @@
     <col min="7" max="8" width="12.6640625" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
     <col min="11" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.83203125" customWidth="1"/>
-    <col min="14" max="14" width="10.1640625" customWidth="1"/>
-    <col min="15" max="15" width="8.1640625" customWidth="1"/>
-    <col min="16" max="16" width="7.6640625" customWidth="1"/>
+    <col min="13" max="13" width="10" customWidth="1"/>
+    <col min="14" max="14" width="12.1640625" customWidth="1"/>
+    <col min="15" max="15" width="9.83203125" customWidth="1"/>
+    <col min="16" max="16" width="10.1640625" customWidth="1"/>
+    <col min="17" max="17" width="8.1640625" customWidth="1"/>
+    <col min="18" max="18" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2313,8 +2328,8 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3">
-        <f>2097152/1024</f>
-        <v>2048</v>
+        <f>1024</f>
+        <v>1024</v>
       </c>
       <c r="B3">
         <v>16</v>
@@ -2378,7 +2393,7 @@
       </c>
       <c r="G7" s="2">
         <f>C7/A3</f>
-        <v>9.765625E-3</v>
+        <v>1.953125E-2</v>
       </c>
       <c r="H7" s="2">
         <f>E7/D7</f>
@@ -2410,7 +2425,7 @@
       </c>
       <c r="G8" s="2">
         <f>C8/A3</f>
-        <v>1.5625E-2</v>
+        <v>3.125E-2</v>
       </c>
       <c r="H8" s="2">
         <f t="shared" ref="H8:H14" si="0">E8/D8</f>
@@ -2442,7 +2457,7 @@
       </c>
       <c r="G9" s="2">
         <f>C9/A3</f>
-        <v>2.4520898437500001E-2</v>
+        <v>4.9041796875000002E-2</v>
       </c>
       <c r="H9" s="2">
         <f t="shared" si="0"/>
@@ -2474,7 +2489,7 @@
       </c>
       <c r="G10" s="2">
         <f>C10/A3</f>
-        <v>3.2546972656249999E-2</v>
+        <v>6.5093945312499998E-2</v>
       </c>
       <c r="H10" s="2">
         <f t="shared" si="0"/>
@@ -2506,7 +2521,7 @@
       </c>
       <c r="G11" s="2">
         <f>C11/A3</f>
-        <v>6.7138671875E-4</v>
+        <v>1.3427734375E-3</v>
       </c>
       <c r="H11" s="2">
         <f t="shared" si="0"/>
@@ -2538,7 +2553,7 @@
       </c>
       <c r="G12" s="2">
         <f>C12/A3</f>
-        <v>7.9345703125E-4</v>
+        <v>1.5869140625E-3</v>
       </c>
       <c r="H12" s="2">
         <f t="shared" si="0"/>
@@ -2570,7 +2585,7 @@
       </c>
       <c r="G13" s="2">
         <f>C13/A3</f>
-        <v>3.1280517578125E-3</v>
+        <v>6.256103515625E-3</v>
       </c>
       <c r="H13" s="2">
         <f t="shared" si="0"/>
@@ -2602,7 +2617,7 @@
       </c>
       <c r="G14" s="2">
         <f>C14/A3</f>
-        <v>3.8299560546875E-3</v>
+        <v>7.659912109375E-3</v>
       </c>
       <c r="H14" s="2">
         <f t="shared" si="0"/>
@@ -2668,7 +2683,7 @@
       </c>
       <c r="G18" s="2">
         <f>C18/A3</f>
-        <v>8.60595703125E-3</v>
+        <v>1.72119140625E-2</v>
       </c>
       <c r="H18" s="2">
         <f>E18/D18</f>
@@ -2700,7 +2715,7 @@
       </c>
       <c r="G19" s="2">
         <f>C19/A3</f>
-        <v>1.3648974609375E-2</v>
+        <v>2.7297949218749999E-2</v>
       </c>
       <c r="H19" s="2">
         <f t="shared" ref="H19:H25" si="2">E19/D19</f>
@@ -2732,7 +2747,7 @@
       </c>
       <c r="G20" s="2">
         <f>C20/A3</f>
-        <v>8.7318359374999998E-3</v>
+        <v>1.7463671875E-2</v>
       </c>
       <c r="H20" s="2">
         <f t="shared" si="2"/>
@@ -2751,7 +2766,7 @@
         <v>37762</v>
       </c>
       <c r="C21">
-        <v>60.484400000000001</v>
+        <v>65.515600000000006</v>
       </c>
       <c r="D21">
         <v>1372785</v>
@@ -2764,7 +2779,7 @@
       </c>
       <c r="G21" s="2">
         <f>C21/A3</f>
-        <v>2.95333984375E-2</v>
+        <v>6.3980078125000006E-2</v>
       </c>
       <c r="H21" s="2">
         <f t="shared" si="2"/>
@@ -2796,7 +2811,7 @@
       </c>
       <c r="G22" s="2">
         <f>C22/A3</f>
-        <v>3.662109375E-4</v>
+        <v>7.32421875E-4</v>
       </c>
       <c r="H22" s="2">
         <f t="shared" si="2"/>
@@ -2828,7 +2843,7 @@
       </c>
       <c r="G23" s="2">
         <f>C23/A3</f>
-        <v>7.171630859375E-4</v>
+        <v>1.434326171875E-3</v>
       </c>
       <c r="H23" s="2">
         <f t="shared" si="2"/>
@@ -2860,7 +2875,7 @@
       </c>
       <c r="G24" s="2">
         <f>C24/A3</f>
-        <v>1.6937255859375E-3</v>
+        <v>3.387451171875E-3</v>
       </c>
       <c r="H24" s="2">
         <f t="shared" si="2"/>
@@ -2892,7 +2907,7 @@
       </c>
       <c r="G25" s="2">
         <f>C25/A3</f>
-        <v>3.6468505859375E-3</v>
+        <v>7.293701171875E-3</v>
       </c>
       <c r="H25" s="2">
         <f t="shared" si="2"/>
@@ -2996,7 +3011,7 @@
       </c>
       <c r="D31">
         <f>C21</f>
-        <v>60.484400000000001</v>
+        <v>65.515600000000006</v>
       </c>
       <c r="E31">
         <f>C20</f>
@@ -3012,7 +3027,7 @@
       </c>
       <c r="H31" s="2">
         <f>D31/B31</f>
-        <v>0.90740846312871126</v>
+        <v>0.9828883134652141</v>
       </c>
       <c r="I31" s="2">
         <f>E31/B31</f>
@@ -3099,7 +3114,7 @@
       </c>
       <c r="H35" s="4">
         <f t="shared" ref="H35:I36" si="6">1/H31</f>
-        <v>1.1020395341608744</v>
+        <v>1.0174095940508825</v>
       </c>
       <c r="I35" s="4">
         <f t="shared" si="6"/>
@@ -3323,7 +3338,7 @@
         <v>767</v>
       </c>
       <c r="F47">
-        <f>SUM(B47:E47)</f>
+        <f t="shared" ref="F47:F52" si="11">SUM(B47:E47)</f>
         <v>1024</v>
       </c>
       <c r="G47" s="3"/>
@@ -3346,7 +3361,7 @@
         <v>488</v>
       </c>
       <c r="F48">
-        <f>SUM(B48:E48)</f>
+        <f t="shared" si="11"/>
         <v>640</v>
       </c>
     </row>
@@ -3367,7 +3382,7 @@
         <v>1763</v>
       </c>
       <c r="F49">
-        <f>SUM(B49:E49)</f>
+        <f t="shared" si="11"/>
         <v>2108</v>
       </c>
     </row>
@@ -3388,7 +3403,7 @@
         <v>28</v>
       </c>
       <c r="F50">
-        <f>SUM(B50:E50)</f>
+        <f t="shared" si="11"/>
         <v>1582</v>
       </c>
     </row>
@@ -3409,7 +3424,7 @@
         <v>251</v>
       </c>
       <c r="F51">
-        <f>SUM(B51:E51)</f>
+        <f t="shared" si="11"/>
         <v>251</v>
       </c>
     </row>
@@ -3430,7 +3445,7 @@
         <v>80</v>
       </c>
       <c r="F52">
-        <f>SUM(B52:E52)</f>
+        <f t="shared" si="11"/>
         <v>205</v>
       </c>
     </row>
@@ -3438,7 +3453,6 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0" footer="0"/>
-  <pageSetup scale="80" fitToHeight="0" pageOrder="overThenDown" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>
@@ -3454,15 +3468,14 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="K48" sqref="K48"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="68" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>